<commit_message>
completed test case TC8
</commit_message>
<xml_diff>
--- a/Test Cases & Observations.xlsx
+++ b/Test Cases & Observations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\morressier-testing-task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FAE78EF-B720-49A5-97E7-C36045E174B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E54B9B-DFBC-4DC3-8BEC-FECEF3DA2DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Observations" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="89">
   <si>
     <t>Expected Results</t>
   </si>
@@ -464,11 +464,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -756,8 +756,8 @@
   <dimension ref="A2:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -918,7 +918,7 @@
       <c r="A9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -936,7 +936,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="10"/>
       <c r="C10" s="5" t="s">
         <v>54</v>
@@ -999,7 +999,9 @@
       <c r="D13" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="5"/>
+      <c r="E13" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
@@ -1012,7 +1014,9 @@
       <c r="D14" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="5"/>
+      <c r="E14" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
@@ -1025,7 +1029,9 @@
       <c r="D15" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="5"/>
+      <c r="E15" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
@@ -1038,7 +1044,9 @@
       <c r="D16" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="5"/>
+      <c r="E16" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
@@ -1051,7 +1059,9 @@
       <c r="D17" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="5"/>
+      <c r="E17" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
     </row>
@@ -1079,7 +1089,9 @@
       <c r="D19" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E19" s="5"/>
+      <c r="E19" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5" t="s">
         <v>86</v>
@@ -1098,7 +1110,9 @@
       <c r="D20" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E20" s="5"/>
+      <c r="E20" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
     </row>
@@ -1176,7 +1190,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF0F1409-08FE-42D0-ADF1-0086244E6DEF}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A2:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -1192,7 +1206,6 @@
     <col min="6" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:5" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>17</v>
@@ -1210,7 +1223,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -1223,7 +1236,7 @@
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" s="6" customFormat="1" ht="69" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="69" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -1236,7 +1249,7 @@
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:5" s="6" customFormat="1" ht="69" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="69" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -1249,7 +1262,7 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" s="6" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -1262,7 +1275,7 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" s="6" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -1275,7 +1288,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -1284,70 +1297,70 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>

</xml_diff>